<commit_message>
little changes in the excel file
</commit_message>
<xml_diff>
--- a/vehicles parameter.xlsx
+++ b/vehicles parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laroc\Desktop\Active_Suspensions_W_Altair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBCC6EB-9954-4BFB-A0F2-5C84C41D98D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329A4438-457E-40CF-BBA9-3CF57E99D2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,24 +42,6 @@
     <t>classic configuration</t>
   </si>
   <si>
-    <t>Sprung mass (ms)</t>
-  </si>
-  <si>
-    <t>Unsprung mass (mus)</t>
-  </si>
-  <si>
-    <t>stiffness of unsprung (kus)</t>
-  </si>
-  <si>
-    <t>stiffness of sprung (ks)</t>
-  </si>
-  <si>
-    <t>dumping of unsprung (cus)</t>
-  </si>
-  <si>
-    <t>dumping of sprung (cs)</t>
-  </si>
-  <si>
     <t>optimization results</t>
   </si>
   <si>
@@ -124,6 +106,24 @@
   </si>
   <si>
     <t xml:space="preserve">supposed mass of unsprung mass </t>
+  </si>
+  <si>
+    <t>Sprung mass (ms) [kg]</t>
+  </si>
+  <si>
+    <t>Unsprung mass (mus) [kg]</t>
+  </si>
+  <si>
+    <t>stiffness of unsprung (kus) [N/m]</t>
+  </si>
+  <si>
+    <t>stiffness of sprung (ks) [N/m]</t>
+  </si>
+  <si>
+    <t>dumping of unsprung (cus) [Ns/m]</t>
+  </si>
+  <si>
+    <t>dumping of sprung (cs) [Ns/m]</t>
   </si>
 </sst>
 </file>
@@ -231,6 +231,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -243,8 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -528,12 +528,12 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
@@ -542,22 +542,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="5"/>
+      <c r="F1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
         <f>G14/4</f>
@@ -568,7 +568,7 @@
         <v>301.25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1">
         <v>1365</v>
@@ -576,7 +576,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
         <f>G15</f>
@@ -587,7 +587,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1">
         <f>G2-(G4*4)</f>
@@ -596,12 +596,12 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1">
         <v>40</v>
@@ -609,14 +609,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -627,34 +627,34 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G9" s="1">
         <v>33.299999999999997</v>
@@ -665,37 +665,37 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="F12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="7"/>
+      <c r="F12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G13" s="1">
         <v>1365</v>
@@ -703,12 +703,12 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1">
         <f>G13-(G15*2)-(G4*2)</f>
@@ -717,12 +717,12 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G15" s="1">
         <f>40+G9</f>
@@ -731,14 +731,14 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>

</xml_diff>